<commit_message>
Added an exception class for cases when the "Joint classes allowed" field in the "Group-TA" sheet of an input file has the wrong format. We also wrote a class for Lab representation
</commit_message>
<xml_diff>
--- a/input_data/Time_Table_Input.xlsx
+++ b/input_data/Time_Table_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10870" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10870" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Group-TA" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="145">
   <si>
     <t>Group Name</t>
   </si>
@@ -641,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -741,12 +741,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -761,6 +763,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -8063,7 +8068,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -16250,7 +16255,7 @@
   </sheetPr>
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -16347,7 +16352,7 @@
   </sheetPr>
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -16458,7 +16463,7 @@
       <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="40">
+      <c r="B12" s="39">
         <v>30</v>
       </c>
       <c r="F12" s="43"/>
@@ -16467,7 +16472,7 @@
       <c r="A13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="40">
+      <c r="B13" s="39">
         <v>30</v>
       </c>
       <c r="F13" s="43"/>
@@ -16476,16 +16481,16 @@
       <c r="A14" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="39">
         <v>30</v>
       </c>
       <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="40">
+      <c r="B15" s="39">
         <v>30</v>
       </c>
       <c r="F15" s="43"/>
@@ -20689,7 +20694,9 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -20704,188 +20711,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="49" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="19" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A2" s="35">
+      <c r="A2" s="47">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="46" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A3" s="35">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A3" s="48"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A4" s="35">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="48"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A5" s="35">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A5" s="48"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A6" s="35">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A6" s="48"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A7" s="35">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>7</v>
-      </c>
+      <c r="A7" s="48"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="41"/>
+      <c r="H7" s="41"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adopted Parsing Algorithm for new input file
</commit_message>
<xml_diff>
--- a/input_data/Time_Table_Input.xlsx
+++ b/input_data/Time_Table_Input.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10870"/>
   </bookViews>
   <sheets>
-    <sheet name="TA-Cours-Groups" sheetId="8" r:id="rId1"/>
+    <sheet name="TA-Course-Groups" sheetId="8" r:id="rId1"/>
     <sheet name="Courses" sheetId="2" r:id="rId2"/>
     <sheet name="Course-Groups" sheetId="7" r:id="rId3"/>
     <sheet name="Teacher Preferences" sheetId="3" r:id="rId4"/>
@@ -682,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,6 +824,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9832,7 +9835,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -9857,8 +9860,8 @@
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="36" t="s">
+    <row r="3" spans="1:2" ht="37.5">
+      <c r="A3" s="52" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="38" t="s">

</xml_diff>

<commit_message>
Validation when user enters not 'Yes' or not 'No' when entering sport electives reservation
</commit_message>
<xml_diff>
--- a/input_data/Time_Table_Input.xlsx
+++ b/input_data/Time_Table_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TA-Course-Groups" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="254">
   <si>
     <t>TA</t>
   </si>
@@ -789,6 +789,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Ye2s</t>
   </si>
 </sst>
 </file>
@@ -2621,7 +2624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ56"/>
   <sheetViews>
-    <sheetView zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -5714,8 +5717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9917,8 +9920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9973,7 +9976,7 @@
         <v>252</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F2" s="39" t="s">
         <v>251</v>

</xml_diff>

<commit_message>
Validation when user enters not 'Offline' or not 'Online' or not '-' when entering format of course
Validation when user enters not 'Full' or not 'Block 1' or not 'Block 2' when entering course type
</commit_message>
<xml_diff>
--- a/input_data/Time_Table_Input.xlsx
+++ b/input_data/Time_Table_Input.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TA-Course-Groups" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="253">
   <si>
     <t>TA</t>
   </si>
@@ -789,9 +789,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>Ye2s</t>
   </si>
 </sst>
 </file>
@@ -2624,8 +2621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ56"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9920,8 +9917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -9976,7 +9973,7 @@
         <v>252</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F2" s="39" t="s">
         <v>251</v>

</xml_diff>